<commit_message>
Convertidos dos aerodromos y actualizada hoja calculo
</commit_message>
<xml_diff>
--- a/airhispania-xsc/AirHispania Aerodromos.xlsx
+++ b/airhispania-xsc/AirHispania Aerodromos.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1682" uniqueCount="1001">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1683" uniqueCount="1003">
   <si>
     <t>GCFV</t>
   </si>
@@ -3040,6 +3040,12 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>si</t>
+  </si>
+  <si>
+    <t>necesario excluir el que tiene xplane para evitar conflictos. Revisar con WED da un problema al cargar</t>
   </si>
 </sst>
 </file>
@@ -3066,7 +3072,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3085,6 +3091,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3098,7 +3116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -3120,6 +3138,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3431,7 +3458,7 @@
   <dimension ref="A1:I287"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A287"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1"/>
@@ -3474,10 +3501,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1">
-      <c r="A2" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>997</v>
       </c>
       <c r="C2" s="1">
@@ -3851,7 +3878,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1">
+    <row r="17" spans="1:9" ht="15" customHeight="1">
       <c r="A17" s="8" t="s">
         <v>1000</v>
       </c>
@@ -3877,7 +3904,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1">
+    <row r="18" spans="1:9" ht="15" customHeight="1">
       <c r="A18" s="8" t="s">
         <v>1000</v>
       </c>
@@ -3903,7 +3930,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1">
+    <row r="19" spans="1:9" ht="15" customHeight="1">
       <c r="A19" s="8" t="s">
         <v>1000</v>
       </c>
@@ -3929,7 +3956,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1">
+    <row r="20" spans="1:9" ht="15" customHeight="1">
       <c r="A20" s="8" t="s">
         <v>1000</v>
       </c>
@@ -3955,7 +3982,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1">
+    <row r="21" spans="1:9" ht="15" customHeight="1">
       <c r="A21" s="8" t="s">
         <v>1000</v>
       </c>
@@ -3981,7 +4008,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15" customHeight="1">
+    <row r="22" spans="1:9" ht="15" customHeight="1">
       <c r="A22" s="8" t="s">
         <v>1000</v>
       </c>
@@ -4007,7 +4034,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1">
+    <row r="23" spans="1:9" ht="15" customHeight="1">
       <c r="A23" s="8" t="s">
         <v>1000</v>
       </c>
@@ -4033,7 +4060,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15" customHeight="1">
+    <row r="24" spans="1:9" ht="15" customHeight="1">
       <c r="A24" s="8" t="s">
         <v>1000</v>
       </c>
@@ -4059,11 +4086,11 @@
         <v>600</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15" customHeight="1">
-      <c r="A25" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B25" s="7" t="s">
+    <row r="25" spans="1:9" ht="15" customHeight="1">
+      <c r="A25" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B25" s="11" t="s">
         <v>997</v>
       </c>
       <c r="C25" s="1">
@@ -4084,8 +4111,11 @@
       <c r="H25" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="15" customHeight="1">
+      <c r="I25" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15" customHeight="1">
       <c r="A26" s="8" t="s">
         <v>1000</v>
       </c>
@@ -4111,7 +4141,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15" customHeight="1">
+    <row r="27" spans="1:9" ht="15" customHeight="1">
       <c r="A27" s="8" t="s">
         <v>1000</v>
       </c>
@@ -4137,7 +4167,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15" customHeight="1">
+    <row r="28" spans="1:9" ht="15" customHeight="1">
       <c r="A28" s="8" t="s">
         <v>1000</v>
       </c>
@@ -4163,7 +4193,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="15" customHeight="1">
+    <row r="29" spans="1:9" ht="15" customHeight="1">
       <c r="A29" s="8" t="s">
         <v>1000</v>
       </c>
@@ -4189,7 +4219,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15" customHeight="1">
+    <row r="30" spans="1:9" ht="15" customHeight="1">
       <c r="A30" s="8" t="s">
         <v>1000</v>
       </c>
@@ -4215,7 +4245,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15" customHeight="1">
+    <row r="31" spans="1:9" ht="15" customHeight="1">
       <c r="A31" s="8" t="s">
         <v>1000</v>
       </c>
@@ -4241,7 +4271,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="15" customHeight="1">
+    <row r="32" spans="1:9" ht="15" customHeight="1">
       <c r="A32" s="8" t="s">
         <v>1000</v>
       </c>

</xml_diff>

<commit_message>
Revisados y convertido AEROVELETA
</commit_message>
<xml_diff>
--- a/airhispania-xsc/AirHispania Aerodromos.xlsx
+++ b/airhispania-xsc/AirHispania Aerodromos.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1683" uniqueCount="1003">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1684" uniqueCount="1004">
   <si>
     <t>GCFV</t>
   </si>
@@ -3045,7 +3045,10 @@
     <t>si</t>
   </si>
   <si>
-    <t>necesario excluir el que tiene xplane para evitar conflictos. Revisar con WED da un problema al cargar</t>
+    <t>Existe en Xplane.es</t>
+  </si>
+  <si>
+    <t>modificar con wed. Las plataformas flotan</t>
   </si>
 </sst>
 </file>
@@ -3458,7 +3461,7 @@
   <dimension ref="A1:I287"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1"/>
@@ -3474,7 +3477,7 @@
     <col min="9" max="9" width="45.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="24.75" customHeight="1">
+    <row r="1" spans="1:9" s="4" customFormat="1" ht="24.75" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>996</v>
       </c>
@@ -3500,7 +3503,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1">
+    <row r="2" spans="1:9" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
         <v>1001</v>
       </c>
@@ -3525,8 +3528,11 @@
       <c r="H2" t="s">
         <v>701</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1">
+      <c r="I2" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
         <v>1000</v>
       </c>
@@ -3552,7 +3558,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1">
+    <row r="4" spans="1:9" ht="15" customHeight="1">
       <c r="A4" s="8" t="s">
         <v>1000</v>
       </c>
@@ -3578,7 +3584,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1">
+    <row r="5" spans="1:9" ht="15" customHeight="1">
       <c r="A5" s="8" t="s">
         <v>1000</v>
       </c>
@@ -3598,7 +3604,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1">
+    <row r="6" spans="1:9" ht="15" customHeight="1">
       <c r="A6" s="8" t="s">
         <v>1000</v>
       </c>
@@ -3606,25 +3612,25 @@
         <v>997</v>
       </c>
       <c r="C6" s="1">
-        <v>-17755611</v>
+        <v>-17887056</v>
       </c>
       <c r="D6" s="1">
-        <v>28626478</v>
+        <v>27814847</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G6" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="H6" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" customHeight="1">
       <c r="A7" s="8" t="s">
         <v>1000</v>
       </c>
@@ -3632,25 +3638,19 @@
         <v>997</v>
       </c>
       <c r="C7" s="1">
-        <v>-15505278</v>
+        <v>-16291852</v>
       </c>
       <c r="D7" s="1">
-        <v>27781111</v>
+        <v>28455019</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" t="s">
-        <v>567</v>
-      </c>
-      <c r="H7" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1">
       <c r="A8" s="8" t="s">
         <v>1000</v>
       </c>
@@ -3658,25 +3658,25 @@
         <v>997</v>
       </c>
       <c r="C8" s="1">
-        <v>-15386586</v>
+        <v>-17755611</v>
       </c>
       <c r="D8" s="1">
-        <v>27931886</v>
+        <v>28626478</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G8" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="H8" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15" customHeight="1">
       <c r="A9" s="8" t="s">
         <v>1000</v>
       </c>
@@ -3684,25 +3684,25 @@
         <v>997</v>
       </c>
       <c r="C9" s="1">
-        <v>-14484667</v>
+        <v>-15505278</v>
       </c>
       <c r="D9" s="1">
-        <v>28086667</v>
+        <v>27781111</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G9" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="H9" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15" customHeight="1">
       <c r="A10" s="8" t="s">
         <v>1000</v>
       </c>
@@ -3710,25 +3710,25 @@
         <v>997</v>
       </c>
       <c r="C10" s="1">
-        <v>-13605225</v>
+        <v>-15386586</v>
       </c>
       <c r="D10" s="1">
-        <v>2894546400000000</v>
+        <v>27931886</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G10" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="H10" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1">
       <c r="A11" s="8" t="s">
         <v>1000</v>
       </c>
@@ -3736,25 +3736,25 @@
         <v>997</v>
       </c>
       <c r="C11" s="1">
-        <v>-16572489</v>
+        <v>-14484667</v>
       </c>
       <c r="D11" s="1">
-        <v>28044475</v>
+        <v>28086667</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F11" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="H11" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15" customHeight="1">
       <c r="A12" s="8" t="s">
         <v>1000</v>
       </c>
@@ -3762,25 +3762,25 @@
         <v>997</v>
       </c>
       <c r="C12" s="1">
-        <v>-16341536</v>
+        <v>-13605225</v>
       </c>
       <c r="D12" s="1">
-        <v>28482653</v>
+        <v>2894546400000000</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>940</v>
+        <v>19</v>
       </c>
       <c r="G12" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="H12" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15" customHeight="1">
       <c r="A13" s="8" t="s">
         <v>1000</v>
       </c>
@@ -3788,25 +3788,25 @@
         <v>997</v>
       </c>
       <c r="C13" s="1">
-        <v>-17887056</v>
+        <v>-16572489</v>
       </c>
       <c r="D13" s="1">
-        <v>27814847</v>
+        <v>28044475</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="G13" t="s">
-        <v>563</v>
+        <v>575</v>
       </c>
       <c r="H13" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15" customHeight="1">
       <c r="A14" s="8" t="s">
         <v>1000</v>
       </c>
@@ -3814,19 +3814,25 @@
         <v>997</v>
       </c>
       <c r="C14" s="1">
-        <v>-16291852</v>
+        <v>-16341536</v>
       </c>
       <c r="D14" s="1">
-        <v>28455019</v>
+        <v>28482653</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1">
+        <v>940</v>
+      </c>
+      <c r="G14" t="s">
+        <v>577</v>
+      </c>
+      <c r="H14" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15" customHeight="1">
       <c r="A15" s="8" t="s">
         <v>1000</v>
       </c>
@@ -3852,7 +3858,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1">
+    <row r="16" spans="1:9" ht="15" customHeight="1">
       <c r="A16" s="8" t="s">
         <v>1000</v>
       </c>
@@ -3879,10 +3885,10 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="15" customHeight="1">
-      <c r="A17" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B17" s="7" t="s">
+      <c r="A17" s="10" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>997</v>
       </c>
       <c r="C17" s="1">
@@ -3902,6 +3908,9 @@
       </c>
       <c r="H17" t="s">
         <v>584</v>
+      </c>
+      <c r="I17" t="s">
+        <v>1003</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15" customHeight="1">
@@ -4090,7 +4099,7 @@
       <c r="A25" s="10" t="s">
         <v>1001</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="9" t="s">
         <v>997</v>
       </c>
       <c r="C25" s="1">
@@ -4111,9 +4120,6 @@
       <c r="H25" t="s">
         <v>602</v>
       </c>
-      <c r="I25" t="s">
-        <v>1002</v>
-      </c>
     </row>
     <row r="26" spans="1:9" ht="15" customHeight="1">
       <c r="A26" s="8" t="s">
@@ -6599,22 +6605,22 @@
         <v>930</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D122" s="1">
-        <v>42571111</v>
+        <v>4093306</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F122" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="G122" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="H122" t="s">
-        <v>751</v>
+        <v>645</v>
       </c>
     </row>
     <row r="123" spans="1:9" ht="15" customHeight="1">
@@ -6625,22 +6631,22 @@
         <v>930</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D123" s="1">
-        <v>39998928</v>
+        <v>42571111</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F123" t="s">
-        <v>950</v>
+        <v>242</v>
       </c>
       <c r="G123" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="H123" t="s">
-        <v>680</v>
+        <v>751</v>
       </c>
     </row>
     <row r="124" spans="1:9" ht="15" customHeight="1">
@@ -6650,23 +6656,23 @@
       <c r="B124" s="7" t="s">
         <v>930</v>
       </c>
-      <c r="C124" s="1">
-        <v>-8377255999999990</v>
+      <c r="C124" s="1" t="s">
+        <v>243</v>
       </c>
       <c r="D124" s="1">
-        <v>43302061</v>
+        <v>39998928</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F124" t="s">
-        <v>246</v>
+        <v>950</v>
       </c>
       <c r="G124" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="H124" t="s">
-        <v>754</v>
+        <v>680</v>
       </c>
       <c r="I124" s="6"/>
     </row>
@@ -6678,22 +6684,22 @@
         <v>930</v>
       </c>
       <c r="C125" s="1">
-        <v>-4386972</v>
+        <v>-8377255999999990</v>
       </c>
       <c r="D125" s="1">
-        <v>39011814</v>
+        <v>43302061</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F125" t="s">
-        <v>954</v>
+        <v>246</v>
       </c>
       <c r="G125" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="H125" t="s">
-        <v>645</v>
+        <v>754</v>
       </c>
     </row>
     <row r="126" spans="1:9" ht="15" customHeight="1">
@@ -6704,22 +6710,22 @@
         <v>930</v>
       </c>
       <c r="C126" s="1">
-        <v>-378306</v>
+        <v>-4386972</v>
       </c>
       <c r="D126" s="1">
-        <v>4038306</v>
+        <v>39011814</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F126" t="s">
-        <v>249</v>
+        <v>954</v>
       </c>
       <c r="G126" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="H126" t="s">
-        <v>757</v>
+        <v>645</v>
       </c>
     </row>
     <row r="127" spans="1:9" ht="15" customHeight="1">
@@ -6730,22 +6736,22 @@
         <v>930</v>
       </c>
       <c r="C127" s="1">
-        <v>-3763351</v>
+        <v>-378306</v>
       </c>
       <c r="D127" s="1">
-        <v>40697159</v>
+        <v>4038306</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F127" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G127" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="H127" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
     </row>
     <row r="128" spans="1:9" ht="15" customHeight="1">
@@ -6755,23 +6761,23 @@
       <c r="B128" s="7" t="s">
         <v>930</v>
       </c>
-      <c r="C128" s="1" t="s">
-        <v>237</v>
+      <c r="C128" s="1">
+        <v>-3763351</v>
       </c>
       <c r="D128" s="1">
-        <v>4093306</v>
+        <v>40697159</v>
       </c>
       <c r="E128" s="2" t="s">
-        <v>238</v>
+        <v>250</v>
       </c>
       <c r="F128" t="s">
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="G128" t="s">
-        <v>749</v>
+        <v>758</v>
       </c>
       <c r="H128" t="s">
-        <v>645</v>
+        <v>759</v>
       </c>
     </row>
     <row r="129" spans="1:8" ht="15" customHeight="1">
@@ -7211,23 +7217,17 @@
       <c r="B146" s="7" t="s">
         <v>998</v>
       </c>
-      <c r="C146" s="1" t="s">
-        <v>991</v>
-      </c>
-      <c r="D146" s="1" t="s">
-        <v>992</v>
+      <c r="C146" s="1">
+        <v>-5695165000000000</v>
+      </c>
+      <c r="D146" s="1">
+        <v>43549761</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>994</v>
+        <v>285</v>
       </c>
       <c r="F146" t="s">
-        <v>993</v>
-      </c>
-      <c r="G146" t="s">
-        <v>989</v>
-      </c>
-      <c r="H146" t="s">
-        <v>990</v>
+        <v>286</v>
       </c>
     </row>
     <row r="147" spans="1:8" ht="15" customHeight="1">
@@ -7237,17 +7237,23 @@
       <c r="B147" s="7" t="s">
         <v>998</v>
       </c>
-      <c r="C147" s="1">
-        <v>-5695165000000000</v>
-      </c>
-      <c r="D147" s="1">
-        <v>43549761</v>
+      <c r="C147" s="1" t="s">
+        <v>991</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>992</v>
       </c>
       <c r="E147" s="2" t="s">
-        <v>285</v>
+        <v>994</v>
       </c>
       <c r="F147" t="s">
-        <v>286</v>
+        <v>993</v>
+      </c>
+      <c r="G147" t="s">
+        <v>989</v>
+      </c>
+      <c r="H147" t="s">
+        <v>990</v>
       </c>
     </row>
     <row r="148" spans="1:8" ht="15" customHeight="1">
@@ -8647,23 +8653,23 @@
       <c r="B207" s="7" t="s">
         <v>998</v>
       </c>
-      <c r="C207" s="1">
-        <v>-1114744</v>
+      <c r="C207" s="1" t="s">
+        <v>398</v>
       </c>
       <c r="D207" s="1">
-        <v>38896378</v>
+        <v>4151667</v>
       </c>
       <c r="E207" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F207" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="G207" t="s">
-        <v>794</v>
+        <v>829</v>
       </c>
       <c r="H207" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="208" spans="1:8" ht="15" customHeight="1">
@@ -8674,22 +8680,22 @@
         <v>998</v>
       </c>
       <c r="C208" s="1">
-        <v>-5655556</v>
+        <v>-1114744</v>
       </c>
       <c r="D208" s="1">
-        <v>42589</v>
+        <v>38896378</v>
       </c>
       <c r="E208" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F208" t="s">
-        <v>969</v>
+        <v>402</v>
       </c>
       <c r="G208" t="s">
-        <v>832</v>
+        <v>794</v>
       </c>
       <c r="H208" t="s">
-        <v>710</v>
+        <v>831</v>
       </c>
     </row>
     <row r="209" spans="1:8" ht="15" customHeight="1">
@@ -8700,22 +8706,22 @@
         <v>998</v>
       </c>
       <c r="C209" s="1">
-        <v>-3320406</v>
+        <v>-5655556</v>
       </c>
       <c r="D209" s="1">
-        <v>39715822</v>
+        <v>42589</v>
       </c>
       <c r="E209" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F209" t="s">
-        <v>405</v>
+        <v>969</v>
       </c>
       <c r="G209" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="H209" t="s">
-        <v>643</v>
+        <v>710</v>
       </c>
     </row>
     <row r="210" spans="1:8" ht="15" customHeight="1">
@@ -8725,23 +8731,23 @@
       <c r="B210" s="7" t="s">
         <v>998</v>
       </c>
-      <c r="C210" s="1" t="s">
-        <v>398</v>
+      <c r="C210" s="1">
+        <v>-3320406</v>
       </c>
       <c r="D210" s="1">
-        <v>4151667</v>
+        <v>39715822</v>
       </c>
       <c r="E210" s="2" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="F210" t="s">
-        <v>400</v>
+        <v>405</v>
       </c>
       <c r="G210" t="s">
-        <v>829</v>
+        <v>833</v>
       </c>
       <c r="H210" t="s">
-        <v>830</v>
+        <v>643</v>
       </c>
     </row>
     <row r="211" spans="1:8" ht="15" customHeight="1">
@@ -10663,7 +10669,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H287"/>
+  <autoFilter ref="A1:H287">
+    <sortState ref="A2:H287">
+      <sortCondition ref="E1:E287"/>
+    </sortState>
+  </autoFilter>
   <sortState ref="A2:I284">
     <sortCondition ref="E154"/>
   </sortState>

</xml_diff>

<commit_message>
mas conversiones y algunas actualizaciones
</commit_message>
<xml_diff>
--- a/airhispania-xsc/AirHispania Aerodromos.xlsx
+++ b/airhispania-xsc/AirHispania Aerodromos.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1685" uniqueCount="1005">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1686" uniqueCount="1006">
   <si>
     <t>GCFV</t>
   </si>
@@ -3048,10 +3048,13 @@
     <t>Existe en Xplane.es</t>
   </si>
   <si>
-    <t>modificar con wed. Las plataformas flotan excluir arboles</t>
-  </si>
-  <si>
     <t xml:space="preserve"> poner taxiways</t>
+  </si>
+  <si>
+    <t>las plataformas flotan</t>
+  </si>
+  <si>
+    <t>modificar con wed. Las plataformas flotan</t>
   </si>
 </sst>
 </file>
@@ -3464,7 +3467,7 @@
   <dimension ref="A1:I287"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1"/>
@@ -3913,7 +3916,7 @@
         <v>584</v>
       </c>
       <c r="I17" t="s">
-        <v>1003</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15" customHeight="1">
@@ -4176,14 +4179,14 @@
         <v>606</v>
       </c>
       <c r="I27" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="15" customHeight="1">
-      <c r="A28" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B28" s="7" t="s">
+      <c r="A28" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>997</v>
       </c>
       <c r="C28" s="1">
@@ -4206,10 +4209,10 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="15" customHeight="1">
-      <c r="A29" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B29" s="7" t="s">
+      <c r="A29" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B29" s="9" t="s">
         <v>997</v>
       </c>
       <c r="C29" s="1">
@@ -4230,12 +4233,15 @@
       <c r="H29" t="s">
         <v>610</v>
       </c>
+      <c r="I29" t="s">
+        <v>1004</v>
+      </c>
     </row>
     <row r="30" spans="1:9" ht="15" customHeight="1">
-      <c r="A30" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B30" s="7" t="s">
+      <c r="A30" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B30" s="9" t="s">
         <v>997</v>
       </c>
       <c r="C30" s="1">
@@ -4284,10 +4290,10 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="15" customHeight="1">
-      <c r="A32" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B32" s="7" t="s">
+      <c r="A32" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B32" s="9" t="s">
         <v>997</v>
       </c>
       <c r="C32" s="1">
@@ -4336,10 +4342,10 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="15" customHeight="1">
-      <c r="A34" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B34" s="7" t="s">
+      <c r="A34" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B34" s="9" t="s">
         <v>997</v>
       </c>
       <c r="C34" s="1">
@@ -4362,10 +4368,10 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="15" customHeight="1">
-      <c r="A35" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B35" s="7" t="s">
+      <c r="A35" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B35" s="9" t="s">
         <v>997</v>
       </c>
       <c r="C35" s="1" t="s">

</xml_diff>

<commit_message>
Agregados aerodromos hechos por Luis y actualizada hoja de calculo
</commit_message>
<xml_diff>
--- a/airhispania-xsc/AirHispania Aerodromos.xlsx
+++ b/airhispania-xsc/AirHispania Aerodromos.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1680" uniqueCount="1007">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1681" uniqueCount="1008">
   <si>
     <t>GCFV</t>
   </si>
@@ -3058,6 +3058,9 @@
   </si>
   <si>
     <t>Tomas</t>
+  </si>
+  <si>
+    <t>En xplane.es</t>
   </si>
 </sst>
 </file>
@@ -3469,8 +3472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A211" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B253" sqref="B253"/>
+    <sheetView tabSelected="1" topLeftCell="A167" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I200" sqref="I200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1"/>
@@ -4734,7 +4737,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="15" customHeight="1">
+    <row r="49" spans="1:9" ht="15" customHeight="1">
       <c r="A49" s="8" t="s">
         <v>1000</v>
       </c>
@@ -4760,7 +4763,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="15" customHeight="1">
+    <row r="50" spans="1:9" ht="15" customHeight="1">
       <c r="A50" s="8" t="s">
         <v>1000</v>
       </c>
@@ -4786,7 +4789,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="15" customHeight="1">
+    <row r="51" spans="1:9" ht="15" customHeight="1">
       <c r="A51" s="8" t="s">
         <v>1000</v>
       </c>
@@ -4812,7 +4815,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="15" customHeight="1">
+    <row r="52" spans="1:9" ht="15" customHeight="1">
       <c r="A52" s="8" t="s">
         <v>1000</v>
       </c>
@@ -4838,7 +4841,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="15" customHeight="1">
+    <row r="53" spans="1:9" ht="15" customHeight="1">
       <c r="A53" s="8" t="s">
         <v>1000</v>
       </c>
@@ -4864,7 +4867,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="15" customHeight="1">
+    <row r="54" spans="1:9" ht="15" customHeight="1">
       <c r="A54" s="8" t="s">
         <v>1000</v>
       </c>
@@ -4890,7 +4893,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="15" customHeight="1">
+    <row r="55" spans="1:9" ht="15" customHeight="1">
       <c r="A55" s="8" t="s">
         <v>1000</v>
       </c>
@@ -4915,8 +4918,11 @@
       <c r="H55" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" ht="15" customHeight="1">
+      <c r="I55" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="15" customHeight="1">
       <c r="A56" s="8" t="s">
         <v>1000</v>
       </c>
@@ -4942,7 +4948,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="15" customHeight="1">
+    <row r="57" spans="1:9" ht="15" customHeight="1">
       <c r="A57" s="8" t="s">
         <v>1000</v>
       </c>
@@ -4968,7 +4974,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="15" customHeight="1">
+    <row r="58" spans="1:9" ht="15" customHeight="1">
       <c r="A58" s="8" t="s">
         <v>1000</v>
       </c>
@@ -4994,7 +5000,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="15" customHeight="1">
+    <row r="59" spans="1:9" ht="15" customHeight="1">
       <c r="A59" s="8" t="s">
         <v>1000</v>
       </c>
@@ -5020,7 +5026,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="15" customHeight="1">
+    <row r="60" spans="1:9" ht="15" customHeight="1">
       <c r="A60" s="8" t="s">
         <v>1000</v>
       </c>
@@ -5046,7 +5052,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="15" customHeight="1">
+    <row r="61" spans="1:9" ht="15" customHeight="1">
       <c r="A61" s="8" t="s">
         <v>1000</v>
       </c>
@@ -5072,7 +5078,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="15" customHeight="1">
+    <row r="62" spans="1:9" ht="15" customHeight="1">
       <c r="A62" s="8" t="s">
         <v>1000</v>
       </c>
@@ -5098,7 +5104,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="15" customHeight="1">
+    <row r="63" spans="1:9" ht="15" customHeight="1">
       <c r="A63" s="8" t="s">
         <v>1000</v>
       </c>
@@ -5124,7 +5130,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="15" customHeight="1">
+    <row r="64" spans="1:9" ht="15" customHeight="1">
       <c r="A64" s="8" t="s">
         <v>1000</v>
       </c>
@@ -5307,10 +5313,10 @@
       </c>
     </row>
     <row r="71" spans="1:8" ht="15" customHeight="1">
-      <c r="A71" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B71" s="7" t="s">
+      <c r="A71" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B71" s="9" t="s">
         <v>930</v>
       </c>
       <c r="C71" s="1">
@@ -5333,10 +5339,10 @@
       </c>
     </row>
     <row r="72" spans="1:8" ht="15" customHeight="1">
-      <c r="A72" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B72" s="7" t="s">
+      <c r="A72" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B72" s="9" t="s">
         <v>930</v>
       </c>
       <c r="C72" s="1">
@@ -5437,10 +5443,10 @@
       </c>
     </row>
     <row r="76" spans="1:8" ht="15" customHeight="1">
-      <c r="A76" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B76" s="7" t="s">
+      <c r="A76" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B76" s="9" t="s">
         <v>930</v>
       </c>
       <c r="C76" s="1">
@@ -5463,10 +5469,10 @@
       </c>
     </row>
     <row r="77" spans="1:8" ht="15" customHeight="1">
-      <c r="A77" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B77" s="7" t="s">
+      <c r="A77" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B77" s="9" t="s">
         <v>930</v>
       </c>
       <c r="C77" s="1">
@@ -5489,10 +5495,10 @@
       </c>
     </row>
     <row r="78" spans="1:8" ht="15" customHeight="1">
-      <c r="A78" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B78" s="7" t="s">
+      <c r="A78" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B78" s="9" t="s">
         <v>930</v>
       </c>
       <c r="C78" s="1">
@@ -5515,10 +5521,10 @@
       </c>
     </row>
     <row r="79" spans="1:8" ht="15" customHeight="1">
-      <c r="A79" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B79" s="7" t="s">
+      <c r="A79" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B79" s="9" t="s">
         <v>930</v>
       </c>
       <c r="C79" s="1">
@@ -5541,10 +5547,10 @@
       </c>
     </row>
     <row r="80" spans="1:8" ht="15" customHeight="1">
-      <c r="A80" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B80" s="7" t="s">
+      <c r="A80" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B80" s="9" t="s">
         <v>930</v>
       </c>
       <c r="C80" s="1" t="s">
@@ -5593,10 +5599,10 @@
       </c>
     </row>
     <row r="82" spans="1:8" ht="15" customHeight="1">
-      <c r="A82" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B82" s="7" t="s">
+      <c r="A82" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B82" s="9" t="s">
         <v>930</v>
       </c>
       <c r="C82" s="1">
@@ -5645,10 +5651,10 @@
       </c>
     </row>
     <row r="84" spans="1:8" ht="15" customHeight="1">
-      <c r="A84" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B84" s="7" t="s">
+      <c r="A84" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B84" s="9" t="s">
         <v>930</v>
       </c>
       <c r="C84" s="1" t="s">
@@ -5671,10 +5677,10 @@
       </c>
     </row>
     <row r="85" spans="1:8" ht="15" customHeight="1">
-      <c r="A85" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B85" s="7" t="s">
+      <c r="A85" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B85" s="9" t="s">
         <v>930</v>
       </c>
       <c r="C85" s="1">
@@ -5723,10 +5729,10 @@
       </c>
     </row>
     <row r="87" spans="1:8" ht="15" customHeight="1">
-      <c r="A87" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B87" s="7" t="s">
+      <c r="A87" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B87" s="9" t="s">
         <v>930</v>
       </c>
       <c r="C87" s="1">
@@ -5749,10 +5755,10 @@
       </c>
     </row>
     <row r="88" spans="1:8" ht="15" customHeight="1">
-      <c r="A88" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B88" s="7" t="s">
+      <c r="A88" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B88" s="9" t="s">
         <v>930</v>
       </c>
       <c r="C88" s="1">
@@ -5775,10 +5781,10 @@
       </c>
     </row>
     <row r="89" spans="1:8" ht="15" customHeight="1">
-      <c r="A89" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B89" s="7" t="s">
+      <c r="A89" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B89" s="9" t="s">
         <v>930</v>
       </c>
       <c r="C89" s="1">
@@ -5801,10 +5807,10 @@
       </c>
     </row>
     <row r="90" spans="1:8" ht="15" customHeight="1">
-      <c r="A90" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B90" s="7" t="s">
+      <c r="A90" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B90" s="9" t="s">
         <v>930</v>
       </c>
       <c r="C90" s="1">
@@ -5827,10 +5833,10 @@
       </c>
     </row>
     <row r="91" spans="1:8" ht="15" customHeight="1">
-      <c r="A91" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B91" s="7" t="s">
+      <c r="A91" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B91" s="9" t="s">
         <v>930</v>
       </c>
       <c r="C91" s="1">
@@ -7096,10 +7102,10 @@
       </c>
     </row>
     <row r="141" spans="1:8" ht="15" customHeight="1">
-      <c r="A141" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B141" s="7" t="s">
+      <c r="A141" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B141" s="9" t="s">
         <v>998</v>
       </c>
       <c r="C141" s="1">
@@ -7122,10 +7128,10 @@
       </c>
     </row>
     <row r="142" spans="1:8" ht="15" customHeight="1">
-      <c r="A142" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B142" s="7" t="s">
+      <c r="A142" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B142" s="9" t="s">
         <v>998</v>
       </c>
       <c r="C142" s="1">
@@ -7148,10 +7154,10 @@
       </c>
     </row>
     <row r="143" spans="1:8" ht="15" customHeight="1">
-      <c r="A143" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B143" s="7" t="s">
+      <c r="A143" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B143" s="9" t="s">
         <v>998</v>
       </c>
       <c r="C143" s="1">
@@ -7174,10 +7180,10 @@
       </c>
     </row>
     <row r="144" spans="1:8" ht="15" customHeight="1">
-      <c r="A144" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B144" s="7" t="s">
+      <c r="A144" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B144" s="9" t="s">
         <v>998</v>
       </c>
       <c r="C144" s="1">
@@ -7900,10 +7906,10 @@
       </c>
     </row>
     <row r="174" spans="1:8" ht="15" customHeight="1">
-      <c r="A174" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B174" s="7" t="s">
+      <c r="A174" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B174" s="9" t="s">
         <v>998</v>
       </c>
       <c r="C174" s="1" t="s">
@@ -7966,10 +7972,10 @@
       </c>
     </row>
     <row r="177" spans="1:8" ht="15" customHeight="1">
-      <c r="A177" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B177" s="7" t="s">
+      <c r="A177" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B177" s="9" t="s">
         <v>998</v>
       </c>
       <c r="C177" s="1" t="s">
@@ -8480,11 +8486,11 @@
       </c>
     </row>
     <row r="200" spans="1:8" ht="15" customHeight="1">
-      <c r="A200" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B200" s="7" t="s">
-        <v>998</v>
+      <c r="A200" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B200" s="9" t="s">
+        <v>1006</v>
       </c>
       <c r="C200" s="1">
         <v>-4289240688</v>
@@ -8558,10 +8564,10 @@
       </c>
     </row>
     <row r="203" spans="1:8" ht="15" customHeight="1">
-      <c r="A203" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B203" s="7" t="s">
+      <c r="A203" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B203" s="9" t="s">
         <v>998</v>
       </c>
       <c r="C203" s="1" t="s">
@@ -8662,10 +8668,10 @@
       </c>
     </row>
     <row r="207" spans="1:8" ht="15" customHeight="1">
-      <c r="A207" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B207" s="7" t="s">
+      <c r="A207" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B207" s="9" t="s">
         <v>998</v>
       </c>
       <c r="C207" s="1">
@@ -8688,10 +8694,10 @@
       </c>
     </row>
     <row r="208" spans="1:8" ht="15" customHeight="1">
-      <c r="A208" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B208" s="7" t="s">
+      <c r="A208" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B208" s="9" t="s">
         <v>998</v>
       </c>
       <c r="C208" s="1">

</xml_diff>

<commit_message>
Agregado enlace a version LEVS Cuatro vientos
</commit_message>
<xml_diff>
--- a/airhispania-xsc/AirHispania Aerodromos.xlsx
+++ b/airhispania-xsc/AirHispania Aerodromos.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1681" uniqueCount="1008">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1682" uniqueCount="1009">
   <si>
     <t>GCFV</t>
   </si>
@@ -3061,6 +3061,9 @@
   </si>
   <si>
     <t>En xplane.es</t>
+  </si>
+  <si>
+    <t>https://mega.co.nz/#F!Dl4gjLba!dGxOtwNQhPBqc2dYeVDxkA</t>
   </si>
 </sst>
 </file>
@@ -3472,8 +3475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I200" sqref="I200"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J127" sqref="J127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1"/>
@@ -3486,7 +3489,7 @@
     <col min="6" max="6" width="33.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="45.7109375" customWidth="1"/>
+    <col min="9" max="9" width="49.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1" ht="24.75" customHeight="1">
@@ -6747,6 +6750,9 @@
       </c>
       <c r="H126" t="s">
         <v>757</v>
+      </c>
+      <c r="I126" t="s">
+        <v>1008</v>
       </c>
     </row>
     <row r="127" spans="1:9" ht="15" customHeight="1">

</xml_diff>

<commit_message>
Actualizada la lista de aerodromos convertidos
</commit_message>
<xml_diff>
--- a/airhispania-xsc/AirHispania Aerodromos.xlsx
+++ b/airhispania-xsc/AirHispania Aerodromos.xlsx
@@ -3171,24 +3171,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -3492,8 +3475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:B50"/>
+    <sheetView tabSelected="1" topLeftCell="A184" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B196" sqref="B196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1"/>
@@ -7249,10 +7232,10 @@
       </c>
     </row>
     <row r="146" spans="1:8" ht="15" customHeight="1">
-      <c r="A146" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B146" s="7" t="s">
+      <c r="A146" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B146" s="9" t="s">
         <v>998</v>
       </c>
       <c r="C146" s="1" t="s">
@@ -7321,10 +7304,10 @@
       </c>
     </row>
     <row r="149" spans="1:8" ht="15" customHeight="1">
-      <c r="A149" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B149" s="7" t="s">
+      <c r="A149" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B149" s="9" t="s">
         <v>998</v>
       </c>
       <c r="C149" s="1">
@@ -7373,10 +7356,10 @@
       </c>
     </row>
     <row r="151" spans="1:8" ht="15" customHeight="1">
-      <c r="A151" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B151" s="7" t="s">
+      <c r="A151" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B151" s="9" t="s">
         <v>998</v>
       </c>
       <c r="C151" s="1">
@@ -7903,10 +7886,10 @@
       </c>
     </row>
     <row r="173" spans="1:8" ht="15" customHeight="1">
-      <c r="A173" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B173" s="7" t="s">
+      <c r="A173" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B173" s="9" t="s">
         <v>998</v>
       </c>
       <c r="C173" s="1">
@@ -8061,10 +8044,10 @@
       </c>
     </row>
     <row r="180" spans="1:8" ht="15" customHeight="1">
-      <c r="A180" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B180" s="7" t="s">
+      <c r="A180" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B180" s="9" t="s">
         <v>998</v>
       </c>
       <c r="C180" s="1">
@@ -8193,10 +8176,10 @@
       </c>
     </row>
     <row r="186" spans="1:8" ht="15" customHeight="1">
-      <c r="A186" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B186" s="7" t="s">
+      <c r="A186" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B186" s="9" t="s">
         <v>998</v>
       </c>
       <c r="C186" s="1">
@@ -8239,10 +8222,10 @@
       </c>
     </row>
     <row r="188" spans="1:8" ht="15" customHeight="1">
-      <c r="A188" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B188" s="7" t="s">
+      <c r="A188" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B188" s="9" t="s">
         <v>998</v>
       </c>
       <c r="C188" s="1">
@@ -8391,10 +8374,10 @@
       </c>
     </row>
     <row r="195" spans="1:8" ht="15" customHeight="1">
-      <c r="A195" s="8" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B195" s="7" t="s">
+      <c r="A195" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B195" s="9" t="s">
         <v>998</v>
       </c>
       <c r="C195" s="1">

</xml_diff>